<commit_message>
api: Well/reagent load: rework for rnai streaming and validation
</commit_message>
<xml_diff>
--- a/db/static/test_data/libraries/clean_data_rnai.xlsx
+++ b/db/static/test_data/libraries/clean_data_rnai.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="data1" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,259 +16,267 @@
     <definedName function="false" hidden="false" name="Excel_BuiltIn_Print_Area_2" vbProcedure="false">data2!$1:$65536</definedName>
     <definedName function="false" hidden="false" name="Excel_BuiltIn_Sheet_Title_1" vbProcedure="false">"data1"</definedName>
     <definedName function="false" hidden="false" name="Excel_BuiltIn_Sheet_Title_2" vbProcedure="false">"data2"</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">#ref!</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Sheet_Title" vbProcedure="false">"data1"</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">#ref!</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Sheet_Title" vbProcedure="false">"data2"</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="81">
-  <si>
-    <t>plate_number</t>
-  </si>
-  <si>
-    <t>well_name</t>
-  </si>
-  <si>
-    <t>library_well_type</t>
-  </si>
-  <si>
-    <t>molar_concentration</t>
-  </si>
-  <si>
-    <t>mg_ml_concentration</t>
-  </si>
-  <si>
-    <t>vendor</t>
-  </si>
-  <si>
-    <t>vendor_reagent_id</t>
-  </si>
-  <si>
-    <t>facility_reagent_id</t>
-  </si>
-  <si>
-    <t>silencing_reagent_type</t>
-  </si>
-  <si>
-    <t>sequence</t>
-  </si>
-  <si>
-    <t>anti_sense_sequence</t>
-  </si>
-  <si>
-    <t>vendor_entrezgene_id</t>
-  </si>
-  <si>
-    <t>vendor_entrezgene_symbols</t>
-  </si>
-  <si>
-    <t>vendor_gene_name</t>
-  </si>
-  <si>
-    <t>vendor_genbank_accession_numbers</t>
-  </si>
-  <si>
-    <t>vendor_species</t>
-  </si>
-  <si>
-    <t>facility_entrezgene_id</t>
-  </si>
-  <si>
-    <t>facility_entrezgene_symbols</t>
-  </si>
-  <si>
-    <t>facility_gene_name</t>
-  </si>
-  <si>
-    <t>facility_genbank_accession_numbers</t>
-  </si>
-  <si>
-    <t>facility_species</t>
-  </si>
-  <si>
-    <t>A05</t>
-  </si>
-  <si>
-    <t>experimental</t>
-  </si>
-  <si>
-    <t>.0001</t>
-  </si>
-  <si>
-    <t>.115</t>
-  </si>
-  <si>
-    <t>vendorX</t>
-  </si>
-  <si>
-    <t>M-005300-00</t>
-  </si>
-  <si>
-    <t>F-005300-00</t>
-  </si>
-  <si>
-    <t>sirna</t>
-  </si>
-  <si>
-    <t>GACAUGCACUGCCUAAUUA;GUACAGAACUCUCCCAUUC;GAUGAAAUGUGCCUUGAAA;GAAGGUGGAUUUGCUAUUG</t>
-  </si>
-  <si>
-    <t>GACAUGCACUGCCUAAUUA;GUACAGAACUCUCCCAUUC;GAUGAAAUGUGCCUUGAAA;GAAGGUGGAUUUGCUAUUA</t>
-  </si>
-  <si>
-    <t>[AAK1;AAK2]</t>
-  </si>
-  <si>
-    <t>VendorGeneNameX</t>
-  </si>
-  <si>
-    <t>[NM_014911;NM_014912]</t>
-  </si>
-  <si>
-    <t>VendorSpeciesX</t>
-  </si>
-  <si>
-    <t>[AAK3;AAK4]</t>
-  </si>
-  <si>
-    <t>FacilityGeneNameX</t>
-  </si>
-  <si>
-    <t>[F_014911;F_014914]</t>
-  </si>
-  <si>
-    <t>FacilitySpeciesX</t>
-  </si>
-  <si>
-    <t>A07</t>
-  </si>
-  <si>
-    <t>library_control</t>
-  </si>
-  <si>
-    <t>M-000000-00</t>
-  </si>
-  <si>
-    <t>GUACAGAGAGGACUACUUC;GGUACGAGGUGAUGCAGUU;UCAGUGGCCUCAACGAGAA;GCAAGUACAGAGAGGACUA</t>
-  </si>
-  <si>
-    <t>GUACAGAGAGGACUACUUC;GGUACGAGGUGAUGCAGUU;UCAGUGGCCUCAACGAGAA;GCAAGUACAGAGAGGACUG</t>
-  </si>
-  <si>
-    <t>[AATK]</t>
-  </si>
-  <si>
-    <t>[XM_375495]</t>
-  </si>
-  <si>
-    <t>A09</t>
-  </si>
-  <si>
-    <t>empty</t>
-  </si>
-  <si>
-    <t>A11</t>
-  </si>
-  <si>
-    <t>rnai_buffer</t>
-  </si>
-  <si>
-    <t>A15</t>
-  </si>
-  <si>
-    <t>.111110</t>
-  </si>
-  <si>
-    <t>10.336</t>
-  </si>
-  <si>
-    <t>M-003256-05</t>
-  </si>
-  <si>
-    <t>GAAAUUGCACUGUCACUAA;CUCAGGAACUCUAUUCUAU;AAACGCCGUCCUUUGAAUA;GCUAAAUCAUCCUUGCAUC</t>
-  </si>
-  <si>
-    <t>GAAAUUGCACUGUCACUAA;CUCAGGAACUCUAUUCUAU;AAACGCCGUCCUUUGAAUA;GCUAAAUCAUCCUUGCAUU</t>
-  </si>
-  <si>
-    <t>[CHEK2]</t>
-  </si>
-  <si>
-    <t>[NM_007194]</t>
-  </si>
-  <si>
-    <t>Plate</t>
-  </si>
-  <si>
-    <t>Well</t>
-  </si>
-  <si>
-    <t>Well Type</t>
-  </si>
-  <si>
-    <t>Concentration</t>
-  </si>
-  <si>
-    <t>Vendor</t>
-  </si>
-  <si>
-    <t>Vendor Reagent ID</t>
-  </si>
-  <si>
-    <t>Facility Reagent ID</t>
-  </si>
-  <si>
-    <t>Silencing Reagent Type</t>
-  </si>
-  <si>
-    <t>Sequences</t>
-  </si>
-  <si>
-    <t>Vendor EntrezGene ID</t>
-  </si>
-  <si>
-    <t>Vendor EntrezGene Symbols</t>
-  </si>
-  <si>
-    <t>Vendor Gene Name</t>
-  </si>
-  <si>
-    <t>Vendor GenBank Accession Numbers</t>
-  </si>
-  <si>
-    <t>Vendor Species</t>
-  </si>
-  <si>
-    <t>Facility EntrezGene ID</t>
-  </si>
-  <si>
-    <t>Facility EntrezGene Symbols</t>
-  </si>
-  <si>
-    <t>Facility Gene Name</t>
-  </si>
-  <si>
-    <t>Facility GenBank Accession Numbers</t>
-  </si>
-  <si>
-    <t>Facility Species</t>
-  </si>
-  <si>
-    <t>Pool Well</t>
-  </si>
-  <si>
-    <t>A20</t>
-  </si>
-  <si>
-    <t>library control</t>
-  </si>
-  <si>
-    <t>M-000000-01</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="82">
+  <si>
+    <t xml:space="preserve">plate_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">well_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">library_well_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">molar_concentration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mg_ml_concentration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vendor_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vendor_reagent_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facility_reagent_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">silencing_reagent_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anti_sense_sequence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vendor_entrezgene_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vendor_entrezgene_symbols</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vendor_gene_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vendor_genbank_accession_numbers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vendor_species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facility_entrezgene_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facility_entrezgene_symbols</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facility_gene_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facility_genbank_accession_numbers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facility_species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">experimental</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.0001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vendorX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M-005300-00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F-005300-00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sirna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GACAUGCACUGCCUAAUUA;GUACAGAACUCUCCCAUUC;GAUGAAAUGUGCCUUGAAA;GAAGGUGGAUUUGCUAUUG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GACAUGCACUGCCUAAUUA;GUACAGAACUCUCCCAUUC;GAUGAAAUGUGCCUUGAAA;GAAGGUGGAUUUGCUAUUA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[AAK1;AAK2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VendorGeneNameX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[NM_014911;NM_014912]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VendorSpeciesX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[AAK3;AAK4]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FacilityGeneNameX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[F_014911;F_014914]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FacilitySpeciesX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">library_control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M-000000-00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GUACAGAGAGGACUACUUC;GGUACGAGGUGAUGCAGUU;UCAGUGGCCUCAACGAGAA;GCAAGUACAGAGAGGACUA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GUACAGAGAGGACUACUUC;GGUACGAGGUGAUGCAGUU;UCAGUGGCCUCAACGAGAA;GCAAGUACAGAGAGGACUG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[AATK]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[XM_375495]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rnai_buffer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.111110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.336</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M-003256-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mirna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GAAAUUGCACUGUCACUAA;CUCAGGAACUCUAUUCUAU;AAACGCCGUCCUUUGAAUA;GCUAAAUCAUCCUUGCAUC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GAAAUUGCACUGUCACUAA;CUCAGGAACUCUAUUCUAU;AAACGCCGUCCUUUGAAUA;GCUAAAUCAUCCUUGCAUU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[CHEK2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[NM_007194]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Well</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Well Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concentration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vendor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vendor Reagent ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facility Reagent ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silencing Reagent Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sequences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vendor EntrezGene ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vendor EntrezGene Symbols</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vendor Gene Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vendor GenBank Accession Numbers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vendor Species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facility EntrezGene ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facility EntrezGene Symbols</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facility Gene Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facility GenBank Accession Numbers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facility Species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pool Well</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">library control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M-000000-01</t>
   </si>
 </sst>
 </file>
@@ -276,7 +284,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
@@ -285,6 +293,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -501,31 +510,31 @@
   </sheetPr>
   <dimension ref="A1:IV6"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.9336734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="11.9336734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="2" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="6" style="2" width="11.9336734693878"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="12.8418367346939"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="14.2551020408163"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="13.5459183673469"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="11.9336734693878"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="11.9336734693878"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="2" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="2" width="13.7142857142857"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="2" width="11.9336734693878"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="13.5459183673469"/>
-    <col collapsed="false" hidden="false" max="256" min="21" style="2" width="11.9336734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="10.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.7448979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="11.7448979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="2" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="6" style="2" width="11.7448979591837"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="11.7448979591837"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="11.7448979591837"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="2" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="2" width="13.5"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="2" width="11.7448979591837"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="256" min="21" style="2" width="11.7448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1960,23 +1969,23 @@
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="9" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L6" s="6" t="n">
         <v>11200</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N6" s="7"/>
       <c r="O6" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
@@ -2244,73 +2253,71 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="8" width="11.530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="20" min="5" style="8" width="11.530612244898"/>
-    <col collapsed="false" hidden="false" max="256" min="21" style="2" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="10.8061224489796"/>
+    <col collapsed="false" hidden="false" max="20" min="1" style="8" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="256" min="21" style="2" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2318,17 +2325,17 @@
         <v>50001</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="11" t="s">
         <v>25</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>

</xml_diff>